<commit_message>
- Added Globe object
- Added Plot object

- Tested initialisation of Globe object

- Made objects flexible so ages and cases can always be specified (not finished)
</commit_message>
<xml_diff>
--- a/structure.xlsx
+++ b/structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B8D894-A2EE-9845-9F6D-3F8DC7FF5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF31AA13-BB1D-F949-B2F2-3D0F1E8A2F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{D43169D5-0DF9-9B4B-8A4F-C5D0D721B1AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Object</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t xml:space="preserve">Contains information on: slab length, world uncertainty, net lithospheric rotation, </t>
+  </si>
+  <si>
+    <t>calculate_world_uncertainty</t>
+  </si>
+  <si>
+    <t>Calculate area of globe at reconstruction age that is preserved in the present-day</t>
   </si>
 </sst>
 </file>
@@ -210,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -311,11 +317,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -328,8 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,7 +683,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,26 +798,44 @@
       <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="D12"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="13"/>
+      <c r="A13" s="10"/>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">

</xml_diff>

<commit_message>
Loads of changes for testing
</commit_message>
<xml_diff>
--- a/structure.xlsx
+++ b/structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF31AA13-BB1D-F949-B2F2-3D0F1E8A2F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EC7AC0-4F94-0A4A-85BA-9D4F56C6EA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{D43169D5-0DF9-9B4B-8A4F-C5D0D721B1AF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{D43169D5-0DF9-9B4B-8A4F-C5D0D721B1AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
-  <si>
-    <t>Object</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Functions</t>
   </si>
@@ -186,13 +183,79 @@
   </si>
   <si>
     <t>Calculate area of globe at reconstruction age that is preserved in the present-day</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>plot_seafloor_age_map</t>
+  </si>
+  <si>
+    <t>plot_sediment_map</t>
+  </si>
+  <si>
+    <t>plot_erosion_rate_map</t>
+  </si>
+  <si>
+    <t>plot_velocity_map</t>
+  </si>
+  <si>
+    <t>plot_velocity_difference_map</t>
+  </si>
+  <si>
+    <t>plot_relative_velocity_difference_map</t>
+  </si>
+  <si>
+    <t>plot_residual_force_map</t>
+  </si>
+  <si>
+    <t>plot_basemap</t>
+  </si>
+  <si>
+    <t>plot_grid</t>
+  </si>
+  <si>
+    <t>plot_vectors</t>
+  </si>
+  <si>
+    <t>plot_reconstruction</t>
+  </si>
+  <si>
+    <t>minimise_residual_torque</t>
+  </si>
+  <si>
+    <t>Optimisation</t>
+  </si>
+  <si>
+    <t>Implemented in test script</t>
+  </si>
+  <si>
+    <t>Function finished</t>
+  </si>
+  <si>
+    <t>Function not finished</t>
+  </si>
+  <si>
+    <t>Function successfully tested</t>
+  </si>
+  <si>
+    <t>calculate_total_subduction_length</t>
+  </si>
+  <si>
+    <t>Calculate the total subduction zone length</t>
+  </si>
+  <si>
+    <t>calculate_number_of_plates</t>
+  </si>
+  <si>
+    <t>Calculate the number of plates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -207,13 +270,45 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -329,10 +424,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -346,8 +443,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,290 +789,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37A9466-00DF-6645-825A-EB9841D856C7}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="101.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="5"/>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12"/>
-      <c r="E12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
+      <c r="E13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
+      <c r="B17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>46</v>
+      <c r="B19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s">
-        <v>22</v>
-      </c>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="5" t="s">
-        <v>39</v>
+      <c r="B22" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="5"/>
+      <c r="A23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
       <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" t="s">
-        <v>30</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="A27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10"/>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="A29" s="10"/>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="A30" s="10"/>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
-      <c r="B31" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
-      <c r="B32" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="10"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="5"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="5"/>
+      <c r="D49" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added saving and exporting to all modules
Successfully initialised PlateTorques object

Restructured initialisation of data and reconstructed_geometries for Plates, Points and Slabs objects.
</commit_message>
<xml_diff>
--- a/structure.xlsx
+++ b/structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EC7AC0-4F94-0A4A-85BA-9D4F56C6EA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695075BB-B9FF-B04A-88C1-79A7400B00D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{D43169D5-0DF9-9B4B-8A4F-C5D0D721B1AF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{D43169D5-0DF9-9B4B-8A4F-C5D0D721B1AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,12 +53,6 @@
     <t>Plates</t>
   </si>
   <si>
-    <t>Reconstruction</t>
-  </si>
-  <si>
-    <t>Stores RotationModel and FeatureCollections (with option to download data directly from the GPlately DataServer)</t>
-  </si>
-  <si>
     <t>ages</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>options</t>
   </si>
   <si>
-    <t>reconstruction</t>
-  </si>
-  <si>
     <t>Resolved topologies and converts them to geopandas.DataFrames. Initialises pandas.DataFrame containing data on plates</t>
   </si>
   <si>
@@ -140,9 +131,6 @@
     <t>calculate_slab_bend_force</t>
   </si>
   <si>
-    <t>plate reconstruction object (gplately.PlateReconstruction)</t>
-  </si>
-  <si>
     <t>Points</t>
   </si>
   <si>
@@ -249,6 +237,18 @@
   </si>
   <si>
     <t>Calculate the number of plates</t>
+  </si>
+  <si>
+    <t>Objects</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Name of the reconstruction, should correspond to identifyer in gplately.DataServer for automatic download</t>
+  </si>
+  <si>
+    <t>Grids</t>
   </si>
 </sst>
 </file>
@@ -311,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -323,17 +323,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -354,19 +343,6 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -429,30 +405,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -789,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37A9466-00DF-6645-825A-EB9841D856C7}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,33 +774,35 @@
     <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="101.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="88.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>25</v>
+      <c r="D2" s="17" t="s">
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
@@ -837,375 +812,386 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="5"/>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
-      <c r="D5" s="5" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="5"/>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="5"/>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="22" t="s">
+      <c r="E12" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="18"/>
+      <c r="B26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31"/>
+    </row>
+    <row r="32" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="17" t="s">
+      <c r="B38" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
-      <c r="B31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="13" t="s">
+      <c r="C49" s="6"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="5"/>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="4"/>
+      <c r="D52" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>